<commit_message>
.ipynb code converted to scripts and added to main file
</commit_message>
<xml_diff>
--- a/docs/Market_Pulse_Data_Dictionary.xlsx
+++ b/docs/Market_Pulse_Data_Dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11400"/>
+    <workbookView windowWidth="25600" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+  <si>
+    <t>Raw Data Fields</t>
+  </si>
   <si>
     <t>Field</t>
   </si>
@@ -65,28 +68,28 @@
     <t>open</t>
   </si>
   <si>
-    <t>INT</t>
-  </si>
-  <si>
-    <t>Opening Price</t>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>Opening Price in USD</t>
   </si>
   <si>
     <t>high</t>
   </si>
   <si>
-    <t>Highest Price</t>
+    <t>Highest price during trading day in USD</t>
   </si>
   <si>
     <t>low</t>
   </si>
   <si>
-    <t>Lowest Price</t>
+    <t>Lowest price during trading day in USD</t>
   </si>
   <si>
     <t>close</t>
   </si>
   <si>
-    <t>Closing Price</t>
+    <t>Closing Price in USD</t>
   </si>
   <si>
     <t>volume</t>
@@ -96,6 +99,51 @@
   </si>
   <si>
     <t>Total Shares Traded</t>
+  </si>
+  <si>
+    <t>Processed Data Fields</t>
+  </si>
+  <si>
+    <t>daily_return</t>
+  </si>
+  <si>
+    <t>data/staged/processed_stocks.csv</t>
+  </si>
+  <si>
+    <t>Log daily return: ln(close_t/close_t-1)</t>
+  </si>
+  <si>
+    <t>volatility_14d</t>
+  </si>
+  <si>
+    <t>14-day rolling volatility (annualized using √252)</t>
+  </si>
+  <si>
+    <t>simple_return</t>
+  </si>
+  <si>
+    <t>Simple daily return: (close_t/close_t-1) - 1</t>
+  </si>
+  <si>
+    <t>cumulative_return</t>
+  </si>
+  <si>
+    <t>Cumulative return from start of period</t>
+  </si>
+  <si>
+    <t>DATA QUALITY NOTES</t>
+  </si>
+  <si>
+    <t>- Missing Values Expected: First row per ticker has NaN daily_return (no previous price)</t>
+  </si>
+  <si>
+    <t>- Rolling Window: First 13 rows per ticker have NaN volatility_14d (insufficient data for 14-day window)</t>
+  </si>
+  <si>
+    <t>- Data Range: Approximately 250 trading days per ticker (one year of market data)</t>
+  </si>
+  <si>
+    <t>- Annualization Factor: Volatility multiplied by √252 to convert daily to annual measure</t>
   </si>
 </sst>
 </file>
@@ -108,9 +156,17 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -589,141 +645,144 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -734,7 +793,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1259,130 +1318,235 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="7" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="7.72727272727273" customWidth="1"/>
+    <col min="1" max="1" width="26.5454545454545" customWidth="1"/>
     <col min="2" max="2" width="9.90909090909091" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="35.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="32.5454545454545" customWidth="1"/>
+    <col min="4" max="4" width="44.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" ht="18.5" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
         <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" ht="18.5" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" ht="18.5" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>